<commit_message>
add cash payment test cases
</commit_message>
<xml_diff>
--- a/test_case/cash_payments/Sumon_Cash_Payment_Test_Cases.xlsx
+++ b/test_case/cash_payments/Sumon_Cash_Payment_Test_Cases.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\test_case_ai_quizwhiz_zluck_com\test_case\cash_payments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0791B64B-8307-44E9-8FC6-2295B8DD4C73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD5C667-9F64-4695-BB3E-F4E3BB3D9FD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tc_Cash_payment" sheetId="1" r:id="rId1"/>
+    <sheet name="Tc_Cash_pay_Functionality" sheetId="2" r:id="rId2"/>
+    <sheet name="Tc_Cash_pay_Security" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="190">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -206,13 +208,454 @@
   </si>
   <si>
     <t>TC-CP-010</t>
+  </si>
+  <si>
+    <t>User on payment page</t>
+  </si>
+  <si>
+    <t>Verify Cash Payment option is displayed</t>
+  </si>
+  <si>
+    <t>1. Go to payment page</t>
+  </si>
+  <si>
+    <t>2. Check payment options</t>
+  </si>
+  <si>
+    <t>Cash Payment option is visible</t>
+  </si>
+  <si>
+    <t>User selects Cash Payment</t>
+  </si>
+  <si>
+    <t>Verify user can select Cash Payment</t>
+  </si>
+  <si>
+    <t>1. Select Cash Payment</t>
+  </si>
+  <si>
+    <t>2. Click Continue</t>
+  </si>
+  <si>
+    <t>Cash Payment selected successfully</t>
+  </si>
+  <si>
+    <t>Verify confirmation message appears</t>
+  </si>
+  <si>
+    <t>2. Confirm order</t>
+  </si>
+  <si>
+    <t>System shows “You have selected Cash Payment”</t>
+  </si>
+  <si>
+    <t>User places order</t>
+  </si>
+  <si>
+    <t>Verify order placed with Cash Payment</t>
+  </si>
+  <si>
+    <t>2. Place order</t>
+  </si>
+  <si>
+    <t>Order placed successfully with status “Pending Payment” or “Cash on Delivery”</t>
+  </si>
+  <si>
+    <t>Verify order summary shows payment type</t>
+  </si>
+  <si>
+    <t>1. Complete cash order</t>
+  </si>
+  <si>
+    <t>2. Check summary</t>
+  </si>
+  <si>
+    <t>Summary shows “Payment Method: Cash”</t>
+  </si>
+  <si>
+    <t>User places multiple orders</t>
+  </si>
+  <si>
+    <t>Verify multiple cash payment orders handled correctly</t>
+  </si>
+  <si>
+    <t>1. Place multiple cash orders</t>
+  </si>
+  <si>
+    <t>Each order is recorded separately</t>
+  </si>
+  <si>
+    <t>Server/API failure</t>
+  </si>
+  <si>
+    <t>Verify error when payment fails to initialize</t>
+  </si>
+  <si>
+    <t>1. Select Cash Payment during server error</t>
+  </si>
+  <si>
+    <t>Error “Unable to process payment” shown</t>
+  </si>
+  <si>
+    <t>Backend check</t>
+  </si>
+  <si>
+    <t>Verify backend logs correct payment type</t>
+  </si>
+  <si>
+    <t>1. Place Cash Payment order</t>
+  </si>
+  <si>
+    <t>2. Check database</t>
+  </si>
+  <si>
+    <t>Payment type logged as “Cash”</t>
+  </si>
+  <si>
+    <t>User cancels order</t>
+  </si>
+  <si>
+    <t>Verify cancellation updates order correctly</t>
+  </si>
+  <si>
+    <t>1. Place Cash order</t>
+  </si>
+  <si>
+    <t>2. Cancel</t>
+  </si>
+  <si>
+    <t>Status updates to “Cancelled”</t>
+  </si>
+  <si>
+    <t>Verify confirmation notification sent</t>
+  </si>
+  <si>
+    <t>2. Check email/SMS</t>
+  </si>
+  <si>
+    <t>Confirmation message received</t>
+  </si>
+  <si>
+    <t>1. Place order</t>
+  </si>
+  <si>
+    <t>CASH_PAY-001</t>
+  </si>
+  <si>
+    <t>CASH_PAY-002</t>
+  </si>
+  <si>
+    <t>CASH_PAY-003</t>
+  </si>
+  <si>
+    <t>CASH_PAY-004</t>
+  </si>
+  <si>
+    <t>CASH_PAY-005</t>
+  </si>
+  <si>
+    <t>CASH_PAY-006</t>
+  </si>
+  <si>
+    <t>CASH_PAY-007</t>
+  </si>
+  <si>
+    <t>CASH_PAY-008</t>
+  </si>
+  <si>
+    <t>CASH_PAY-009</t>
+  </si>
+  <si>
+    <t>Verify HTTPS is enforced on the payment page</t>
+  </si>
+  <si>
+    <t>1. Open payment page</t>
+  </si>
+  <si>
+    <t>2. Observe the URL</t>
+  </si>
+  <si>
+    <t>Payment page must load using HTTPS, not HTTP</t>
+  </si>
+  <si>
+    <t>User placing order</t>
+  </si>
+  <si>
+    <t>Verify secure transmission of payment-related data</t>
+  </si>
+  <si>
+    <t>1. Place a cash payment order</t>
+  </si>
+  <si>
+    <t>2. Inspect network requests</t>
+  </si>
+  <si>
+    <t>Sensitive data (order ID, user info) must be encrypted in transit</t>
+  </si>
+  <si>
+    <t>SEC_CASH003</t>
+  </si>
+  <si>
+    <t>User logged in</t>
+  </si>
+  <si>
+    <t>Verify session timeout during inactivity</t>
+  </si>
+  <si>
+    <t>1. Log in</t>
+  </si>
+  <si>
+    <t>2. Stay idle for a long period</t>
+  </si>
+  <si>
+    <t>3. Try to place order</t>
+  </si>
+  <si>
+    <t>System should log out or prompt re-login before payment</t>
+  </si>
+  <si>
+    <t>SEC_CASH004</t>
+  </si>
+  <si>
+    <t>Verify CSRF token is present for cash payment form</t>
+  </si>
+  <si>
+    <t>1. Inspect form request</t>
+  </si>
+  <si>
+    <t>2. Look for CSRF token</t>
+  </si>
+  <si>
+    <t>Request must contain valid CSRF token to prevent cross-site attacks</t>
+  </si>
+  <si>
+    <t>SEC_CASH005</t>
+  </si>
+  <si>
+    <t>Payment form visible</t>
+  </si>
+  <si>
+    <t>Verify XSS prevention in cash payment fields</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;script&gt;alert(‘XSS’)&lt;/script&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in address or note field</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Submit payment</t>
+  </si>
+  <si>
+    <t>Input must be sanitized; no script should execute</t>
+  </si>
+  <si>
+    <t>SEC_CASH006</t>
+  </si>
+  <si>
+    <t>Verify SQL injection prevention in address or note field</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>' OR 1=1 --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in input fields</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Submit order</t>
+  </si>
+  <si>
+    <t>System must reject or sanitize input</t>
+  </si>
+  <si>
+    <t>SEC_CASH007</t>
+  </si>
+  <si>
+    <t>User account created</t>
+  </si>
+  <si>
+    <t>Verify duplicate cash order submission is blocked</t>
+  </si>
+  <si>
+    <t>1. Click “Place Order” multiple times quickly</t>
+  </si>
+  <si>
+    <t>Only one order should be created</t>
+  </si>
+  <si>
+    <t>SEC_CASH008</t>
+  </si>
+  <si>
+    <t>Verify unauthorized user cannot access payment endpoint</t>
+  </si>
+  <si>
+    <t>1. Log out</t>
+  </si>
+  <si>
+    <t>2. Try to access payment URL directly</t>
+  </si>
+  <si>
+    <t>System should redirect to login page or show “Unauthorized Access”</t>
+  </si>
+  <si>
+    <t>SEC_CASH009</t>
+  </si>
+  <si>
+    <t>Order placed with cash payment</t>
+  </si>
+  <si>
+    <t>Verify sensitive information (like phone, address) is masked in logs</t>
+  </si>
+  <si>
+    <t>2. Review backend logs</t>
+  </si>
+  <si>
+    <t>Logs must not contain full personal data</t>
+  </si>
+  <si>
+    <t>SEC_CASH010</t>
+  </si>
+  <si>
+    <t>Verify server logs don’t store plaintext payment info</t>
+  </si>
+  <si>
+    <t>1. Check application logs</t>
+  </si>
+  <si>
+    <t>No sensitive info (user data, token) should be stored in plain text</t>
+  </si>
+  <si>
+    <t>SEC_CASH011</t>
+  </si>
+  <si>
+    <t>Admin panel access</t>
+  </si>
+  <si>
+    <t>Verify access control for cash payment details</t>
+  </si>
+  <si>
+    <t>1. Login as user with limited access</t>
+  </si>
+  <si>
+    <t>2. Try to view all orders</t>
+  </si>
+  <si>
+    <t>Access should be denied for unauthorized roles</t>
+  </si>
+  <si>
+    <t>SEC_CASH012</t>
+  </si>
+  <si>
+    <t>Payment endpoint active</t>
+  </si>
+  <si>
+    <t>Verify API request validation for cash payment</t>
+  </si>
+  <si>
+    <t>1. Try sending malformed API request for cash order</t>
+  </si>
+  <si>
+    <t>API should reject request and return validation error</t>
+  </si>
+  <si>
+    <t>SEC_CASH013</t>
+  </si>
+  <si>
+    <t>Payment confirmation email</t>
+  </si>
+  <si>
+    <t>Verify no sensitive data is leaked via email</t>
+  </si>
+  <si>
+    <t>1. Complete order</t>
+  </si>
+  <si>
+    <t>2. Check confirmation email</t>
+  </si>
+  <si>
+    <t>Email should not contain sensitive payment or user info</t>
+  </si>
+  <si>
+    <t>SEC_CASH014</t>
+  </si>
+  <si>
+    <t>User session active</t>
+  </si>
+  <si>
+    <t>Verify payment session expires after successful order</t>
+  </si>
+  <si>
+    <t>1. Place cash order</t>
+  </si>
+  <si>
+    <t>2. Reload payment URL</t>
+  </si>
+  <si>
+    <t>Payment session/token should be invalid after completion</t>
+  </si>
+  <si>
+    <t>SEC_CASH015</t>
+  </si>
+  <si>
+    <t>Admin user</t>
+  </si>
+  <si>
+    <t>Verify audit log records cash payment operations</t>
+  </si>
+  <si>
+    <t>2. Check admin audit logs</t>
+  </si>
+  <si>
+    <t>Audit should record who placed the order, when, and from which IP</t>
+  </si>
+  <si>
+    <t>TC_SECU_001</t>
+  </si>
+  <si>
+    <t>TC_SECU_002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +679,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -251,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -349,13 +806,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,15 +869,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,237 +1244,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -981,4 +1482,968 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC1E828-5F08-455E-AE6D-BF606FE2D205}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="50">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC4511A-AC1D-4D46-B47D-0EEB8B08410A}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" ht="43.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" ht="29.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="14"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="71">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cash payment test cases
</commit_message>
<xml_diff>
--- a/test_case/cash_payments/Sumon_Cash_Payment_Test_Cases.xlsx
+++ b/test_case/cash_payments/Sumon_Cash_Payment_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\test_case_ai_quizwhiz_zluck_com\test_case\cash_payments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD5C667-9F64-4695-BB3E-F4E3BB3D9FD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716C767B-8490-4104-8DB9-D142EFB3322A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1227,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>

</xml_diff>